<commit_message>
Finalized cost calculator spreadsheet, better carousel images, changed carousel styling.
</commit_message>
<xml_diff>
--- a/public/files/disinfectantcostcalculator.xlsx
+++ b/public/files/disinfectantcostcalculator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="21075" windowHeight="11325" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="21075" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="RTU Wipes" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>Disinfectant Cost Calculator</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>Concentrates</t>
+  </si>
+  <si>
+    <t>Ounces per Container:</t>
+  </si>
+  <si>
+    <t>Dilution Ratio (eg if 1:16, enter 16)</t>
+  </si>
+  <si>
+    <t>Cost Per Concentrated Ounce:</t>
+  </si>
+  <si>
+    <t>Cost Per In-Use Gallon:</t>
   </si>
 </sst>
 </file>
@@ -112,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,27 +141,30 @@
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -194,28 +209,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -520,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,214 +551,318 @@
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="11">
+      <c r="E6" s="2"/>
+      <c r="F6" s="8">
         <v>9966125</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="9">
         <v>100</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7">
+      <c r="C8" s="7"/>
+      <c r="D8" s="9">
         <v>150</v>
       </c>
-      <c r="F8" s="7">
+      <c r="E8" s="2"/>
+      <c r="F8" s="9">
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="10">
         <v>12</v>
       </c>
-      <c r="D10" s="1">
+      <c r="C10" s="2"/>
+      <c r="D10" s="10">
         <v>12</v>
       </c>
-      <c r="F10" s="1">
+      <c r="E10" s="2"/>
+      <c r="F10" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="10">
         <v>160</v>
       </c>
-      <c r="D12" s="1">
+      <c r="C12" s="2"/>
+      <c r="D12" s="10">
         <v>150</v>
       </c>
-      <c r="F12" s="1">
+      <c r="E12" s="2"/>
+      <c r="F12" s="10">
         <v>250</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="11">
         <f>B8/B10/B12</f>
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11">
         <f t="shared" ref="D14:F14" si="0">D8/D10/D12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="10">
         <v>20</v>
       </c>
-      <c r="D18" s="1">
+      <c r="C18" s="2"/>
+      <c r="D18" s="10">
         <v>15</v>
       </c>
-      <c r="F18" s="1">
+      <c r="E18" s="2"/>
+      <c r="F18" s="10">
         <v>8</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="11">
         <f>B14*B18</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11">
         <f t="shared" ref="D20:F20" si="1">D14*D18</f>
         <v>1.25</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8">
+      <c r="E20" s="11"/>
+      <c r="F20" s="11">
         <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="1">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="10">
         <v>100</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="11">
         <f>B20*D22</f>
         <v>104.16666666666667</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="8">
+      <c r="C24" s="14"/>
+      <c r="D24" s="11">
         <f>D20*D22</f>
         <v>125</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="8">
+      <c r="E24" s="14"/>
+      <c r="F24" s="11">
         <f>F20*D22</f>
         <v>64</v>
       </c>
     </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="11">
         <f>B24*365</f>
         <v>38020.833333333336</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11">
         <f t="shared" ref="D26:F26" si="2">D24*365</f>
         <v>45625</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8">
+      <c r="E26" s="11"/>
+      <c r="F26" s="11">
         <f t="shared" si="2"/>
         <v>23360</v>
       </c>
@@ -754,10 +875,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,246 +891,359 @@
     <col min="6" max="6" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="11">
+      <c r="E6" s="2"/>
+      <c r="F6" s="8">
         <v>9966125</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="9">
         <v>100</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7">
+      <c r="C8" s="7"/>
+      <c r="D8" s="9">
         <v>150</v>
       </c>
-      <c r="F8" s="7">
+      <c r="E8" s="2"/>
+      <c r="F8" s="9">
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="10">
         <v>12</v>
       </c>
-      <c r="D10" s="1">
+      <c r="C10" s="2"/>
+      <c r="D10" s="10">
         <v>12</v>
       </c>
-      <c r="F10" s="1">
+      <c r="E10" s="2"/>
+      <c r="F10" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="10">
         <v>160</v>
       </c>
-      <c r="D12" s="1">
+      <c r="C12" s="2"/>
+      <c r="D12" s="10">
         <v>150</v>
       </c>
-      <c r="F12" s="1">
+      <c r="E12" s="2"/>
+      <c r="F12" s="10">
         <v>250</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="11">
         <f>B8/B10/B12</f>
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11">
         <f t="shared" ref="D14:F14" si="0">D8/D10/D12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="10">
         <v>20</v>
       </c>
-      <c r="D16" s="1">
+      <c r="C16" s="2"/>
+      <c r="D16" s="10">
         <v>15</v>
       </c>
-      <c r="F16" s="1">
+      <c r="E16" s="2"/>
+      <c r="F16" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="9">
         <v>0.2</v>
       </c>
-      <c r="D18" s="7">
+      <c r="C18" s="2"/>
+      <c r="D18" s="9">
         <v>0.3</v>
       </c>
-      <c r="F18" s="7">
+      <c r="E18" s="2"/>
+      <c r="F18" s="9">
         <v>0.3</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="10">
         <v>20</v>
       </c>
-      <c r="D20" s="1">
+      <c r="C20" s="2"/>
+      <c r="D20" s="10">
         <v>10</v>
       </c>
-      <c r="F20" s="1">
+      <c r="E20" s="2"/>
+      <c r="F20" s="10">
         <v>10</v>
       </c>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="11">
         <f>B14*B16+B18*B20</f>
         <v>5.041666666666667</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11">
         <f t="shared" ref="D22:F22" si="1">D14*D16+D18*D20</f>
         <v>4.25</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8">
+      <c r="E22" s="11"/>
+      <c r="F22" s="11">
         <f t="shared" si="1"/>
         <v>3.64</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="1">
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="10">
         <v>100</v>
       </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="11">
         <f>B22*D24</f>
         <v>504.16666666666669</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="8">
+      <c r="C26" s="14"/>
+      <c r="D26" s="11">
         <f>D22*D24</f>
         <v>425</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="8">
+      <c r="E26" s="14"/>
+      <c r="F26" s="11">
         <f>F22*D24</f>
         <v>364</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="11">
         <f>B26*365</f>
         <v>184020.83333333334</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11">
         <f t="shared" ref="D28:F28" si="2">D26*365</f>
         <v>155125</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8">
+      <c r="E28" s="11"/>
+      <c r="F28" s="11">
         <f t="shared" si="2"/>
         <v>132860</v>
       </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1018,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,219 +1268,381 @@
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="11">
+      <c r="E6" s="2"/>
+      <c r="F6" s="8">
         <v>9966125</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="9">
         <v>100</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7">
+      <c r="C8" s="7"/>
+      <c r="D8" s="9">
         <v>150</v>
       </c>
-      <c r="F8" s="7">
+      <c r="E8" s="2"/>
+      <c r="F8" s="9">
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="10">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="10">
         <v>12</v>
       </c>
-      <c r="D10" s="1">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="E10" s="2"/>
+      <c r="F10" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1">
-        <v>160</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="10">
+        <v>128</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="10">
         <v>150</v>
       </c>
-      <c r="F12" s="1">
+      <c r="E12" s="2"/>
+      <c r="F12" s="10">
         <v>250</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="8">
+      <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="11">
         <f>B8/B10/B12</f>
-        <v>5.2083333333333336E-2</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8">
+        <v>0.13020833333333334</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11">
         <f t="shared" ref="D14:F14" si="0">D8/D10/D12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="1">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="12">
+        <v>16</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12">
+        <v>256</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="11">
+        <f>256/(B16+1)*B14</f>
+        <v>1.9607843137254903</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11">
+        <f t="shared" ref="D18:F18" si="1">256/(D16+1)*D14</f>
+        <v>8.3009079118028531E-2</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11">
+        <f t="shared" si="1"/>
+        <v>0.62060606060606061</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="10">
         <v>20</v>
       </c>
-      <c r="D18" s="1">
+      <c r="C22" s="2"/>
+      <c r="D22" s="10">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="11">
+        <f>B18+B20*B22</f>
+        <v>5.9607843137254903</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11">
+        <f t="shared" ref="C24:F24" si="2">D18+D20*D22</f>
+        <v>3.0830090791180287</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11">
+        <f t="shared" si="2"/>
+        <v>3.6206060606060606</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="10">
+        <v>100</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="8">
-        <f>B14*B18</f>
-        <v>1.0416666666666667</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8">
-        <f t="shared" ref="D20:F20" si="1">D14*D18</f>
-        <v>1.25</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8">
-        <f t="shared" si="1"/>
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="1">
-        <v>100</v>
-      </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="8">
-        <f>B20*D22</f>
-        <v>104.16666666666667</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="8">
-        <f>D20*D22</f>
-        <v>125</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="8">
-        <f>F20*D22</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B28" s="11">
+        <f>B24*D26</f>
+        <v>596.07843137254906</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="11">
+        <f>D24*D26</f>
+        <v>308.30090791180288</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="11">
+        <f>F24*D26</f>
+        <v>362.06060606060606</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="8">
-        <f>B24*365</f>
-        <v>38020.833333333336</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8">
-        <f t="shared" ref="D26:F26" si="2">D24*365</f>
-        <v>45625</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8">
-        <f t="shared" si="2"/>
-        <v>23360</v>
+      <c r="B30" s="11">
+        <f>B28*365</f>
+        <v>217568.62745098042</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11">
+        <f t="shared" ref="D30:F30" si="3">D28*365</f>
+        <v>112529.83138780805</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11">
+        <f t="shared" si="3"/>
+        <v>132152.12121212122</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>